<commit_message>
Memoria TP6 casi terminada, cambios minimos en el codigo
</commit_message>
<xml_diff>
--- a/tp6-parte2/comparacion_laplace.xlsx
+++ b/tp6-parte2/comparacion_laplace.xlsx
@@ -228,12 +228,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -244,6 +238,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:G18"/>
+  <dimension ref="C1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,285 +541,302 @@
   <sheetData>
     <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="9"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0.9849</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>0.98360000000000003</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0.98529999999999995</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="10">
+      <c r="C5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.98660000000000003</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.98550000000000004</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.98829999999999996</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.98719999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="8">
         <v>0.3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" s="3">
         <v>0.98599999999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="4">
         <v>0.9849</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F6" s="3">
         <v>0.98780000000000001</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G6" s="4">
         <v>0.98660000000000003</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="10">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="8">
         <v>0.6</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="3">
         <v>0.98580000000000001</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E7" s="4">
         <v>0.98450000000000004</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="3">
         <v>0.98709999999999998</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G7" s="4">
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="10">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="8">
         <v>0.9</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="3">
         <v>0.98560000000000003</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E8" s="4">
         <v>0.98429999999999995</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F8" s="3">
         <v>0.9869</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G8" s="4">
         <v>0.98570000000000002</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="10">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D9" s="3">
         <v>0.98509999999999998</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E9" s="4">
         <v>0.98380000000000001</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="3">
         <v>0.98699999999999999</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G9" s="4">
         <v>0.9859</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="10">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="8">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="3">
         <v>0.98419999999999996</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E10" s="4">
         <v>0.98260000000000003</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="3">
         <v>0.98560000000000003</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G10" s="4">
         <v>0.98419999999999996</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="10">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D11" s="3">
         <v>0.96750000000000003</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E11" s="4">
         <v>0.96330000000000005</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F11" s="3">
         <v>0.98370000000000002</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G11" s="4">
         <v>0.98209999999999997</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="10">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="8">
         <v>7</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="3">
         <v>0.93420000000000003</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E12" s="4">
         <v>0.92249999999999999</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F12" s="3">
         <v>0.98050000000000004</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G12" s="4">
         <v>0.97850000000000004</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="10">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="8">
         <v>9</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="3">
         <v>0.89100000000000001</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E13" s="4">
         <v>0.86480000000000001</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F13" s="3">
         <v>0.97750000000000004</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G13" s="4">
         <v>0.9728</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="10">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="8">
         <v>15</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="3">
         <v>0.7722</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E14" s="4">
         <v>0.66859999999999997</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F14" s="3">
         <v>0.95379999999999998</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G14" s="4">
         <v>0.94720000000000004</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="10">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="8">
         <v>20</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D15" s="3">
         <v>0.69369999999999998</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E15" s="4">
         <v>0.49640000000000001</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F15" s="3">
         <v>0.93559999999999999</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G15" s="4">
         <v>0.92479999999999996</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="10">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="8">
         <v>35</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D16" s="3">
         <v>0.5867</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E16" s="4">
         <v>0.17530000000000001</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F16" s="3">
         <v>0.88939999999999997</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G16" s="4">
         <v>0.8629</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="10">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="8">
         <v>50</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="3">
         <v>0.56330000000000002</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E17" s="4">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F17" s="3">
         <v>0.85580000000000001</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G17" s="4">
         <v>0.81330000000000002</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="11">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="9">
         <v>75</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="3">
         <v>0.54679999999999995</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E18" s="4">
         <v>1.7299999999999999E-2</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F18" s="3">
         <v>0.81599999999999995</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G18" s="4">
         <v>0.74850000000000005</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="12">
+    <row r="19" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="10">
         <v>100</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D19" s="5">
         <v>0.54290000000000005</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E19" s="6">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F19" s="5">
         <v>0.78590000000000004</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G19" s="6">
         <v>0.69479999999999997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Memoria del TP6 finalizada. Comprimido creado.
</commit_message>
<xml_diff>
--- a/tp6-parte2/comparacion_laplace.xlsx
+++ b/tp6-parte2/comparacion_laplace.xlsx
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:G19"/>
+  <dimension ref="C1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,256 +587,273 @@
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D5" s="3">
-        <v>0.98660000000000003</v>
+        <v>0.98719999999999997</v>
       </c>
       <c r="E5" s="4">
-        <v>0.98550000000000004</v>
+        <v>0.98609999999999998</v>
       </c>
       <c r="F5" s="3">
-        <v>0.98829999999999996</v>
+        <v>0.98819999999999997</v>
       </c>
       <c r="G5" s="4">
-        <v>0.98719999999999997</v>
+        <v>0.98709999999999998</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="8">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="3">
-        <v>0.98599999999999999</v>
+        <v>0.98660000000000003</v>
       </c>
       <c r="E6" s="4">
-        <v>0.9849</v>
+        <v>0.98550000000000004</v>
       </c>
       <c r="F6" s="3">
-        <v>0.98780000000000001</v>
+        <v>0.98829999999999996</v>
       </c>
       <c r="G6" s="4">
-        <v>0.98660000000000003</v>
+        <v>0.98719999999999997</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="8">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D7" s="3">
-        <v>0.98580000000000001</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="E7" s="4">
-        <v>0.98450000000000004</v>
+        <v>0.9849</v>
       </c>
       <c r="F7" s="3">
-        <v>0.98709999999999998</v>
+        <v>0.98780000000000001</v>
       </c>
       <c r="G7" s="4">
-        <v>0.98599999999999999</v>
+        <v>0.98660000000000003</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="8">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D8" s="3">
-        <v>0.98560000000000003</v>
+        <v>0.98580000000000001</v>
       </c>
       <c r="E8" s="4">
-        <v>0.98429999999999995</v>
+        <v>0.98450000000000004</v>
       </c>
       <c r="F8" s="3">
-        <v>0.9869</v>
+        <v>0.98709999999999998</v>
       </c>
       <c r="G8" s="4">
-        <v>0.98570000000000002</v>
+        <v>0.98599999999999999</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D9" s="3">
-        <v>0.98509999999999998</v>
+        <v>0.98560000000000003</v>
       </c>
       <c r="E9" s="4">
-        <v>0.98380000000000001</v>
+        <v>0.98429999999999995</v>
       </c>
       <c r="F9" s="3">
-        <v>0.98699999999999999</v>
+        <v>0.9869</v>
       </c>
       <c r="G9" s="4">
-        <v>0.9859</v>
+        <v>0.98570000000000002</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>0.98419999999999996</v>
+        <v>0.98509999999999998</v>
       </c>
       <c r="E10" s="4">
-        <v>0.98260000000000003</v>
+        <v>0.98380000000000001</v>
       </c>
       <c r="F10" s="3">
-        <v>0.98560000000000003</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="G10" s="4">
-        <v>0.98419999999999996</v>
+        <v>0.9859</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="3">
-        <v>0.96750000000000003</v>
+        <v>0.98419999999999996</v>
       </c>
       <c r="E11" s="4">
-        <v>0.96330000000000005</v>
+        <v>0.98260000000000003</v>
       </c>
       <c r="F11" s="3">
-        <v>0.98370000000000002</v>
+        <v>0.98560000000000003</v>
       </c>
       <c r="G11" s="4">
-        <v>0.98209999999999997</v>
+        <v>0.98419999999999996</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
-        <v>0.93420000000000003</v>
+        <v>0.96750000000000003</v>
       </c>
       <c r="E12" s="4">
-        <v>0.92249999999999999</v>
+        <v>0.96330000000000005</v>
       </c>
       <c r="F12" s="3">
-        <v>0.98050000000000004</v>
+        <v>0.98370000000000002</v>
       </c>
       <c r="G12" s="4">
-        <v>0.97850000000000004</v>
+        <v>0.98209999999999997</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" s="8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3">
-        <v>0.89100000000000001</v>
+        <v>0.93420000000000003</v>
       </c>
       <c r="E13" s="4">
-        <v>0.86480000000000001</v>
+        <v>0.92249999999999999</v>
       </c>
       <c r="F13" s="3">
-        <v>0.97750000000000004</v>
+        <v>0.98050000000000004</v>
       </c>
       <c r="G13" s="4">
-        <v>0.9728</v>
+        <v>0.97850000000000004</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" s="8">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3">
-        <v>0.7722</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="E14" s="4">
-        <v>0.66859999999999997</v>
+        <v>0.86480000000000001</v>
       </c>
       <c r="F14" s="3">
-        <v>0.95379999999999998</v>
+        <v>0.97750000000000004</v>
       </c>
       <c r="G14" s="4">
-        <v>0.94720000000000004</v>
+        <v>0.9728</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15" s="8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3">
-        <v>0.69369999999999998</v>
+        <v>0.7722</v>
       </c>
       <c r="E15" s="4">
-        <v>0.49640000000000001</v>
+        <v>0.66859999999999997</v>
       </c>
       <c r="F15" s="3">
-        <v>0.93559999999999999</v>
+        <v>0.95379999999999998</v>
       </c>
       <c r="G15" s="4">
-        <v>0.92479999999999996</v>
+        <v>0.94720000000000004</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" s="8">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D16" s="3">
-        <v>0.5867</v>
+        <v>0.69369999999999998</v>
       </c>
       <c r="E16" s="4">
-        <v>0.17530000000000001</v>
+        <v>0.49640000000000001</v>
       </c>
       <c r="F16" s="3">
-        <v>0.88939999999999997</v>
+        <v>0.93559999999999999</v>
       </c>
       <c r="G16" s="4">
-        <v>0.8629</v>
+        <v>0.92479999999999996</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="8">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.5867</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.17530000000000001</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.88939999999999997</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.8629</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="8">
         <v>50</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D18" s="3">
         <v>0.56330000000000002</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E18" s="4">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F18" s="3">
         <v>0.85580000000000001</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G18" s="4">
         <v>0.81330000000000002</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="9">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="9">
         <v>75</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D19" s="3">
         <v>0.54679999999999995</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="4">
         <v>1.7299999999999999E-2</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F19" s="3">
         <v>0.81599999999999995</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G19" s="4">
         <v>0.74850000000000005</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="10">
+    <row r="20" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="10">
         <v>100</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D20" s="5">
         <v>0.54290000000000005</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E20" s="6">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F20" s="5">
         <v>0.78590000000000004</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G20" s="6">
         <v>0.69479999999999997</v>
       </c>
     </row>

</xml_diff>